<commit_message>
Added final submission PDF
</commit_message>
<xml_diff>
--- a/Lab5/Results.xlsx
+++ b/Lab5/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tux\UF\CompArch\Labs\EEL5764_ComputerArch_UF\Lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A46D4A-90CE-4641-81C3-E0AFFE8D2FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D024DF6-5344-4B6C-816F-6E83DEB233FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{81EAA817-A6D1-46E6-9FAB-28C4F48F4DD6}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>numIQEntries</t>
-  </si>
-  <si>
-    <t>Ticks</t>
   </si>
   <si>
     <t>LQEntries</t>
@@ -151,13 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,247 +471,247 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>5</v>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>1740727000</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="3">
         <v>999611000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="3">
         <v>3150472000</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1">
         <v>196777000</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1">
         <v>196777000</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>32</v>
       </c>
       <c r="B3" s="3">
         <v>215399000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>16</v>
       </c>
       <c r="E3" s="3">
         <v>221875000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>48</v>
       </c>
       <c r="H3" s="3">
         <v>247485000</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="J3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="1">
         <v>199791000</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="M3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="1">
         <v>121770000</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>48</v>
       </c>
       <c r="B4" s="3">
         <v>191046000</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="3">
         <v>194339000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>96</v>
       </c>
       <c r="H4" s="3">
         <v>197370000</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1">
         <v>196872000</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="1">
         <v>106493000</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>64</v>
       </c>
       <c r="B5" s="3">
         <v>187681000</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>32</v>
       </c>
       <c r="E5" s="3">
         <v>187681000</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>192</v>
       </c>
       <c r="H5" s="3">
         <v>187681000</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="J5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1">
         <v>207582000</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="1">
         <v>103301000</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>96</v>
       </c>
       <c r="B6" s="3">
         <v>187681000</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>48</v>
       </c>
       <c r="E6" s="3">
         <v>187549000</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>288</v>
       </c>
       <c r="H6" s="3">
         <v>187549000</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1">
         <v>211481000</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>128</v>
       </c>
       <c r="B7" s="3">
         <v>187681000</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>64</v>
       </c>
       <c r="E7" s="3">
         <v>187549000</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>384</v>
       </c>
       <c r="H7" s="3">
         <v>187549000</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1">
+        <v>200191000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="2">
-        <v>200191000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>207844000</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="J9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1">
         <v>211617000</v>
       </c>
     </row>

</xml_diff>